<commit_message>
Excel actualizado con la nueva columna.
</commit_message>
<xml_diff>
--- a/ESP_37_23-24_Villarreal-Real_Madrid_tiros.xlsx
+++ b/ESP_37_23-24_Villarreal-Real_Madrid_tiros.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M34"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,55 +446,60 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>localia</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>minuto</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>xg</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>zona_contacto</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>resultado</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>y</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>situacion</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>asistente</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>accion_anterior</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>id</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>partido</t>
         </is>
@@ -511,53 +516,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>5</v>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>0.07621308416128159</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>0.8530000305175781</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>0.590999984741211</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J2" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
           <t>Alexander Sørloth</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M2" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -574,53 +584,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>5</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
         <v>0.01734926924109459</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Tiro al palo</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>0.7190000152587891</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>0.4159999847412109</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J3" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>Santiago Comesaña</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="L3" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M3" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -637,53 +652,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
         <v>9</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>0.03300964087247849</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>0.8830000305175781</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>0.285</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J4" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
           <t>Gerard Moreno</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M4" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -700,49 +720,54 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>9</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
         <v>0.04186709225177765</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>0.785</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>0.5279999923706055</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr">
         <is>
           <t>Perdida</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M5" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -759,53 +784,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>17</v>
       </c>
-      <c r="D6" t="n">
+      <c r="E6" t="n">
         <v>0.01993104629218578</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Tiro a porteria</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>0.88</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>0.38299999237060545</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J6" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
           <t>Alberto Moreno</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M6" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -822,53 +852,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
         <v>19</v>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>0.02653988264501095</v>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>0.8480000305175781</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>0.255</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J7" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
           <t>Daniel Parejo</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr">
+      <c r="L7" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M7" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -885,53 +920,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>22</v>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>0.06734903156757355</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>0.8490000152587891</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>0.5990000152587891</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J8" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
           <t>Alberto Moreno</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M8" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -948,53 +988,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
         <v>22</v>
       </c>
-      <c r="D9" t="n">
+      <c r="E9" t="n">
         <v>0.1218038350343704</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>Tiro a porteria</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>0.9519999694824218</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>0.5670000076293945</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Remate de corner</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
+      <c r="K9" t="inlineStr">
         <is>
           <t>Daniel Parejo</t>
         </is>
       </c>
-      <c r="K9" t="inlineStr">
+      <c r="L9" t="inlineStr">
         <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M9" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1011,53 +1056,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
         <v>38</v>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>0.09630098193883896</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>0.904000015258789</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>0.51</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J10" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
           <t>Yerson Mosquera</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M10" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1074,53 +1124,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
         <v>42</v>
       </c>
-      <c r="D11" t="n">
+      <c r="E11" t="n">
         <v>0.06447101384401321</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>0.914000015258789</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>0.475</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J11" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
           <t>Gonçalo Guedes</t>
         </is>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="L11" t="inlineStr">
         <is>
           <t>Aereo</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M11" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1137,53 +1192,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
         <v>47</v>
       </c>
-      <c r="D12" t="n">
+      <c r="E12" t="n">
         <v>0.3369220793247223</v>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>0.919000015258789</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>0.5120000076293946</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J12" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
           <t>Gerard Moreno</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M12" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1200,53 +1260,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
         <v>48</v>
       </c>
-      <c r="D13" t="n">
+      <c r="E13" t="n">
         <v>0.07832451164722443</v>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t>0.8480000305175781</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>0.40599998474121096</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J13" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
           <t>Gerard Moreno</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M13" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1263,53 +1328,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>51</v>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>0.07537191361188889</v>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>0.87</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>0.40200000762939453</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J14" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
           <t>Gerard Moreno</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M14" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1326,49 +1396,54 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
         <v>51</v>
       </c>
-      <c r="D15" t="n">
+      <c r="E15" t="n">
         <v>0.3395519852638245</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>0.9059999847412109</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>0.445</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr">
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr">
         <is>
           <t>Rechace</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M15" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1385,53 +1460,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
         <v>53</v>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>0.07688968628644943</v>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>0.894000015258789</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>0.5270000076293946</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J16" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
           <t>Alberto Moreno</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="L16" t="inlineStr">
         <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M16" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1448,53 +1528,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
         <v>55</v>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>0.5439315438270569</v>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>0.8980000305175782</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>0.5590000152587891</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
           <t>Gerard Moreno</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr">
+      <c r="L17" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M17" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1511,49 +1596,54 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
         <v>57</v>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>0.0218716636300087</v>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>0.7959999847412109</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>0.73</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr"/>
-      <c r="K18" t="inlineStr">
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr">
         <is>
           <t>Regate</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M18" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1570,45 +1660,50 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
         <v>70</v>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>0.02152775414288044</v>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>0.7819999694824219</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>0.40900001525878904</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>Balon parado</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1625,45 +1720,50 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
         <v>81</v>
       </c>
-      <c r="D20" t="n">
+      <c r="E20" t="n">
         <v>0.08722219616174698</v>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>0.9030000305175782</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>0.49700000762939456</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr"/>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
       <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1680,53 +1780,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
         <v>82</v>
       </c>
-      <c r="D21" t="n">
+      <c r="E21" t="n">
         <v>0.05989894270896912</v>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>0.9119999694824219</t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t>0.47200000762939454</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J21" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
           <t>Gonçalo Guedes</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>Aereo</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M21" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1743,53 +1848,58 @@
           <t>Villarreal</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
         <v>89</v>
       </c>
-      <c r="D22" t="n">
+      <c r="E22" t="n">
         <v>0.03102139011025429</v>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Tiro a porteria</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>0.894000015258789</t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t>0.27</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J22" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
           <t>Gonçalo Guedes</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M22" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1806,53 +1916,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>8</v>
       </c>
-      <c r="D23" t="n">
+      <c r="E23" t="n">
         <v>0.0117569463327527</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>Tiro a porteria</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>0.6980000305175781</t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t>0.6719999694824219</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J23" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
           <t>Dani Ceballos</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>Recuperacion</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M23" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1869,53 +1984,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>12</v>
       </c>
-      <c r="D24" t="n">
+      <c r="E24" t="n">
         <v>0.01909618265926838</v>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>0.7330000305175781</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t>0.3370000076293945</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>Remate de corner</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
+      <c r="K24" t="inlineStr">
         <is>
           <t>Dani Ceballos</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M24" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1932,53 +2052,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
         <v>13</v>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>0.3808590769767761</v>
       </c>
-      <c r="E25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>0.874000015258789</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t>0.549000015258789</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J25" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
           <t>Brahim Diaz</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M25" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -1995,53 +2120,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
         <v>17</v>
       </c>
-      <c r="D26" t="n">
+      <c r="E26" t="n">
         <v>0.03939567878842354</v>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>Tiro a porteria</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>0.7809999847412109</t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t>0.509000015258789</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J26" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
           <t>Luka Modric</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="L26" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M26" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2058,53 +2188,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
         <v>29</v>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>0.4369303584098816</v>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>0.9580000305175781</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t>0.42900001525878906</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J27" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
           <t>Lucas Vázquez</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="L27" t="inlineStr">
         <is>
           <t>Centro</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M27" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2121,53 +2256,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
         <v>39</v>
       </c>
-      <c r="D28" t="n">
+      <c r="E28" t="n">
         <v>0.136467456817627</v>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>0.8919999694824219</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t>0.5709999847412109</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J28" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
           <t>Brahim Diaz</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="L28" t="inlineStr">
         <is>
           <t>Pase en profundidad</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M28" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2184,53 +2324,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
         <v>43</v>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>0.01423274353146553</v>
       </c>
-      <c r="E29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>Cabeza</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>0.8690000152587891</t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>0.505</t>
         </is>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>Remate de corner</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>Luka Modric</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>Aereo</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M29" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2247,53 +2392,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>46</v>
       </c>
-      <c r="D30" t="n">
+      <c r="E30" t="n">
         <v>0.3145969212055206</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>Gol</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>0.9440000152587891</t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t>0.3579999923706055</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J30" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
           <t>Lucas Vázquez</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="L30" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M30" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2310,53 +2460,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>49</v>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>0.03117688372731209</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>0.7809999847412109</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t>0.35900001525878905</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J31" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
           <t>Lucas Vázquez</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr">
+      <c r="L31" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M31" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2373,53 +2528,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>62</v>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>0.03529926389455795</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>Pierna izquierda</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>Tiro fuera</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>0.85</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t>0.29</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J32" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
           <t>Luka Modric</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>Regate</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M32" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2436,53 +2596,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
         <v>63</v>
       </c>
-      <c r="D33" t="n">
+      <c r="E33" t="n">
         <v>0.06410320103168488</v>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>Tiro bloqueado</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>0.8590000152587891</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t>0.34400001525878904</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J33" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
           <t>Arda Güler</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="L33" t="inlineStr">
         <is>
           <t>Pase</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M33" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>
@@ -2499,53 +2664,58 @@
           <t>Real Madrid</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>visitante</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
         <v>78</v>
       </c>
-      <c r="D34" t="n">
+      <c r="E34" t="n">
         <v>0.1073756739497185</v>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>Pierna derecha</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>Tiro al palo</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>0.965</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t>0.34</t>
         </is>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>Juego abierto</t>
-        </is>
-      </c>
       <c r="J34" t="inlineStr">
         <is>
+          <t>Juego abierto</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
           <t>Eduardo Camavinga</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="L34" t="inlineStr">
         <is>
           <t>Regate</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
-        </is>
-      </c>
       <c r="M34" t="inlineStr">
+        <is>
+          <t>La_liga_37_23-24_Villarreal-Real Madrid</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
         <is>
           <t>Villarreal-Real Madrid</t>
         </is>

</xml_diff>